<commit_message>
Added nozzles, rigids for equipment, more stuff...
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39185D70-009E-412F-838D-7260C7F74EFE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13B4DE3-A344-404B-9C1E-181D5D2976E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="PIPELINES" sheetId="11" r:id="rId7"/>
     <sheet name="ELEMENTS" sheetId="12" r:id="rId8"/>
     <sheet name="SUPPORTS" sheetId="13" r:id="rId9"/>
+    <sheet name="PROFILES" sheetId="15" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="188">
   <si>
     <t>TMONT</t>
   </si>
@@ -545,7 +546,58 @@
     <t>CW</t>
   </si>
   <si>
-    <t>94</t>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Pipe Types: Rigid</t>
+  </si>
+  <si>
+    <t>PROF</t>
+  </si>
+  <si>
+    <t>_RIGID_</t>
+  </si>
+  <si>
+    <t>ACHSE</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>EQUIPMENT</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>LQX</t>
+  </si>
+  <si>
+    <t>LQY</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>LQZ</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>LMX</t>
+  </si>
+  <si>
+    <t>LMY</t>
+  </si>
+  <si>
+    <t>LMZ</t>
+  </si>
+  <si>
+    <t>13.35</t>
+  </si>
+  <si>
+    <t>2.55</t>
   </si>
 </sst>
 </file>
@@ -942,6 +994,138 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31859DAF-9455-4D9E-AE4A-F6AD039EC19C}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.42578125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <picture r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
@@ -1010,15 +1194,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,6 +1260,34 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2031,10 +2244,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2258,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -2061,8 +2274,26 @@
       <c r="E1" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>88</v>
       </c>
@@ -2076,7 +2307,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>91</v>
       </c>
@@ -2087,7 +2318,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
@@ -2098,7 +2329,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -2109,7 +2340,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>96</v>
       </c>
@@ -2120,7 +2351,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -2131,7 +2362,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -2142,7 +2373,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
@@ -2153,7 +2384,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>101</v>
       </c>
@@ -2164,7 +2395,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>102</v>
       </c>
@@ -2175,7 +2406,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>103</v>
       </c>
@@ -2186,7 +2417,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -2197,7 +2428,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>100</v>
       </c>
@@ -2208,7 +2439,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>107</v>
       </c>
@@ -2219,7 +2450,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -2230,7 +2461,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>108</v>
       </c>
@@ -2241,7 +2472,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>113</v>
       </c>
@@ -2251,8 +2482,26 @@
       <c r="D18" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -2263,7 +2512,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>115</v>
       </c>
@@ -2274,7 +2523,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -2285,7 +2534,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>117</v>
       </c>
@@ -2296,7 +2545,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>118</v>
       </c>
@@ -2307,7 +2556,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -2318,7 +2567,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>120</v>
       </c>
@@ -2329,7 +2578,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -2340,7 +2589,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -2351,7 +2600,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -2362,7 +2611,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>156</v>
       </c>
@@ -2373,7 +2622,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>130</v>
       </c>
@@ -2384,7 +2633,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>153</v>
       </c>
@@ -2395,7 +2644,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -2461,7 +2710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update config file for Madumvej
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\Revit-PCF-Exporter\revit-ntr-exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5986A1A2-D504-44DA-8517-AC7F552913F8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C8CBAC-CC1B-4BB4-ABD8-B7694512720C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="204">
   <si>
     <t>TMONT</t>
   </si>
@@ -613,6 +613,39 @@
   </si>
   <si>
     <t>94</t>
+  </si>
+  <si>
+    <t>BROEN BALLOMAX: 200 FG Håndhjul</t>
+  </si>
+  <si>
+    <t>39.1</t>
+  </si>
+  <si>
+    <t>66.8</t>
+  </si>
+  <si>
+    <t>Flowserve_V726DKONA_DN150: DN 150</t>
+  </si>
+  <si>
+    <t>Flowserve_V726DKVNA_DN80: DN 80</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>SONO3300_PN40: DN150</t>
+  </si>
+  <si>
+    <t>SONO3300_PN40: DN200</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>54</t>
   </si>
 </sst>
 </file>
@@ -648,13 +681,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2259,10 +2293,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,7 +2522,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2517,7 +2551,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2528,7 +2562,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2539,7 +2573,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2550,7 +2584,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2561,7 +2595,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2572,146 +2606,201 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>119</v>
+      <c r="A24" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>138</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>120</v>
+      <c r="A25" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>127</v>
+      <c r="A26" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>128</v>
+      <c r="A27" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>129</v>
+      <c r="A28" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>156</v>
+      <c r="A29" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>130</v>
+      <c r="A30" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>153</v>
+      <c r="A31" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>154</v>
+      <c r="A32" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>161</v>
+      <c r="A33" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>162</v>
+      <c r="A34" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>163</v>
+      <c r="A35" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>164</v>
+      <c r="A36" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>155</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change some NORM stuff
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5986A1A2-D504-44DA-8517-AC7F552913F8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6FBB7F-7DC1-44B2-BA8A-A4A7F396AAD6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GEN" sheetId="1" r:id="rId1"/>
@@ -369,9 +369,6 @@
     <t>'EN 10253-2 - Type B'</t>
   </si>
   <si>
-    <t>'EN 10253-2'</t>
-  </si>
-  <si>
     <t>'EN 1092-1/11/PN40'</t>
   </si>
   <si>
@@ -613,6 +610,9 @@
   </si>
   <si>
     <t>94</t>
+  </si>
+  <si>
+    <t>'EN 10253-2 - Type A'</t>
   </si>
 </sst>
 </file>
@@ -994,7 +994,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -1039,7 +1039,7 @@
         <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>84</v>
@@ -1047,22 +1047,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1293,16 +1293,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1315,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2261,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2281,7 @@
         <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -2290,22 +2290,22 @@
         <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2330,7 +2330,7 @@
         <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2341,7 +2341,7 @@
         <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2352,7 +2352,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
         <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2374,7 +2374,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2385,7 +2385,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>105</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
         <v>105</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2429,7 +2429,7 @@
         <v>105</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
         <v>105</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2451,7 +2451,7 @@
         <v>105</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2473,7 +2473,7 @@
         <v>109</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2484,234 +2484,234 @@
         <v>109</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>111</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2725,7 +2725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2743,141 +2743,141 @@
         <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final update to component file and remove it...
</commit_message>
<xml_diff>
--- a/revit-ntr-exporter/NTR_CONFIG.xlsx
+++ b/revit-ntr-exporter/NTR_CONFIG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Revit-PCF-Exporter\Revit-NTR-Exporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6FBB7F-7DC1-44B2-BA8A-A4A7F396AAD6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0A71B1-3A20-4085-B2E6-67A11E96B0BF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="204">
   <si>
     <t>TMONT</t>
   </si>
@@ -513,9 +513,6 @@
     <t>20</t>
   </si>
   <si>
-    <t>'Madumvej-2018.05.18'</t>
-  </si>
-  <si>
     <t>W-filter: DN 150</t>
   </si>
   <si>
@@ -613,6 +610,42 @@
   </si>
   <si>
     <t>'EN 10253-2 - Type A'</t>
+  </si>
+  <si>
+    <t>SONO3300_PN40: DN150</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>SONO3300_PN40: DN200</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Flowserve_V726DKONA_DN150: DN 150</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>Flowserve_V726DKVNA_DN80: DN 80</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>39.1</t>
+  </si>
+  <si>
+    <t>BROEN BALLOMAX: 200 FG Håndhjul</t>
+  </si>
+  <si>
+    <t>66.8</t>
+  </si>
+  <si>
+    <t>'Madumvej-2018.05.30'</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1072,7 @@
         <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>84</v>
@@ -1047,22 +1080,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1161,7 +1194,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1293,16 +1326,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2259,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,22 +2323,22 @@
         <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2462,7 +2495,7 @@
         <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2473,7 +2506,7 @@
         <v>109</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2484,7 +2517,7 @@
         <v>109</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2498,26 +2531,26 @@
         <v>111</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I18" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2528,7 +2561,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -2539,7 +2572,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2550,7 +2583,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2561,7 +2594,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2572,146 +2605,201 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>118</v>
+      <c r="A24" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>119</v>
+      <c r="A25" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>138</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>126</v>
+      <c r="A26" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>127</v>
+      <c r="A27" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>128</v>
+      <c r="A28" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>155</v>
+      <c r="A29" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>129</v>
+      <c r="A30" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>152</v>
+      <c r="A31" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>153</v>
+      <c r="A32" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>160</v>
+      <c r="A33" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>161</v>
+      <c r="A34" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>162</v>
+      <c r="A35" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>163</v>
+      <c r="A36" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>154</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2749,7 +2837,7 @@
         <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2825,18 +2913,18 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>141</v>
@@ -2844,29 +2932,29 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>141</v>
@@ -2874,7 +2962,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>141</v>

</xml_diff>